<commit_message>
feat: Aktifkan menu pengaturan akun dengan upload foto profil
- Tambah halaman pengaturan-akun.html untuk upload foto profil
- Update dashboard-siswa.html untuk navigasi ke pengaturan akun
- Tambah migration_add_photo_url.sql untuk kolom photo_url
- Tambah PANDUAN_PENGATURAN_AKUN.md untuk setup guide
- Fitur: upload foto (JPEG/PNG max 2MB), preview, validasi
- Integrasi dengan Supabase Storage untuk penyimpanan foto
- Fallback ke UI Avatars jika belum upload foto
</commit_message>
<xml_diff>
--- a/DAFTAR NAMA SISWA KELAS X-XII 2026.xlsx
+++ b/DAFTAR NAMA SISWA KELAS X-XII 2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplikasi Web AI\LP Kokulikuler SMAN 1 Belitang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2478DD-7709-4324-9F6F-9AD73C69C58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003D917C-25FE-4737-B245-847895FF5C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29815,8 +29815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:F353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B345"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>